<commit_message>
Match manually corrected SpeciesSeeded column to subplot data
</commit_message>
<xml_diff>
--- a/data/raw/03.1b_edited-species-seeded1_corrected-seeded-not-in-mix_subplot.xlsx
+++ b/data/raw/03.1b_edited-species-seeded1_corrected-seeded-not-in-mix_subplot.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{E4B6624F-F1D1-4948-BE4F-D27FFF9DA9DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="104" documentId="13_ncr:40009_{E4B6624F-F1D1-4948-BE4F-D27FFF9DA9DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8EA6864-194B-40E0-B1E6-F75F26780712}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={B2899F8C-4835-4657-A201-9626AE43BAA8}</author>
   </authors>
   <commentList>
-    <comment ref="E59" authorId="0" shapeId="0">
+    <comment ref="E60" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="166">
   <si>
     <t>Site</t>
   </si>
@@ -521,13 +521,28 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>SRER</t>
+  </si>
+  <si>
+    <t>Sonoran SE</t>
+  </si>
+  <si>
+    <t>BOUSPP</t>
+  </si>
+  <si>
+    <t>BOUSPP.SRER</t>
+  </si>
+  <si>
+    <t>Bouteloua spp., SRER</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -661,12 +676,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="34">
@@ -1081,16 +1090,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>847725</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>565784</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>24765</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>243840</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>468629</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>20955</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1105,8 +1114,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11028045" y="533400"/>
-          <a:ext cx="2802255" cy="1485900"/>
+          <a:off x="11729084" y="567690"/>
+          <a:ext cx="3560445" cy="3072765"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1146,7 +1155,43 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> only corrected if plant was identified to genus level and definitely not seeded.  Unknowns retain original classification.</a:t>
+            <a:t> only corrected if:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>- Plant was identified to genus level and definitely not seeded. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>- Named "local Bouteloua" because if it's local I think that implies a volunteer, and also because the same name was used at other sites and marked not seeded. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>- Marked "Yes?" - I just took away question mark.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>- An unknown and not specifically marked as seeded. I need to change these because otherwise they conflict with the lists of the unknowns and the not seeded, and creates duplicates when using left_join() on </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>corrected species seeding data and subplot data.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1469,18 +1514,19 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="E59" dT="2023-09-07T00:11:45.05" personId="{8230C25F-1289-450E-882A-C133D8E3F471}" id="{B2899F8C-4835-4657-A201-9626AE43BAA8}">
+  <threadedComment ref="E60" dT="2023-09-07T00:11:45.05" personId="{8230C25F-1289-450E-882A-C133D8E3F471}" id="{B2899F8C-4835-4657-A201-9626AE43BAA8}">
     <text>USDA code is actually LILE29</text>
   </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J76"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J57" sqref="J57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1540,7 +1586,7 @@
       <c r="D2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F2" t="s">
@@ -1555,8 +1601,8 @@
       <c r="I2" t="s">
         <v>17</v>
       </c>
-      <c r="J2" t="s">
-        <v>18</v>
+      <c r="J2" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -1572,7 +1618,7 @@
       <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F3" t="s">
@@ -1587,8 +1633,8 @@
       <c r="I3" t="s">
         <v>17</v>
       </c>
-      <c r="J3" t="s">
-        <v>18</v>
+      <c r="J3" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -1604,7 +1650,7 @@
       <c r="D4" t="s">
         <v>20</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F4" t="s">
@@ -1619,8 +1665,8 @@
       <c r="I4" t="s">
         <v>17</v>
       </c>
-      <c r="J4" t="s">
-        <v>18</v>
+      <c r="J4" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -1636,7 +1682,7 @@
       <c r="D5" t="s">
         <v>23</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F5" t="s">
@@ -1651,8 +1697,8 @@
       <c r="I5" t="s">
         <v>26</v>
       </c>
-      <c r="J5" t="s">
-        <v>18</v>
+      <c r="J5" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -1668,7 +1714,7 @@
       <c r="D6" t="s">
         <v>27</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F6" t="s">
@@ -1683,8 +1729,8 @@
       <c r="I6" t="s">
         <v>17</v>
       </c>
-      <c r="J6" t="s">
-        <v>18</v>
+      <c r="J6" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -1700,7 +1746,7 @@
       <c r="D7" t="s">
         <v>27</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F7" t="s">
@@ -1715,8 +1761,8 @@
       <c r="I7" t="s">
         <v>17</v>
       </c>
-      <c r="J7" t="s">
-        <v>18</v>
+      <c r="J7" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -1732,7 +1778,7 @@
       <c r="D8" t="s">
         <v>30</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F8" t="s">
@@ -1747,8 +1793,8 @@
       <c r="I8" t="s">
         <v>34</v>
       </c>
-      <c r="J8" t="s">
-        <v>18</v>
+      <c r="J8" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -1764,7 +1810,7 @@
       <c r="D9" t="s">
         <v>38</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="1" t="s">
         <v>39</v>
       </c>
       <c r="F9" t="s">
@@ -1779,8 +1825,8 @@
       <c r="I9" t="s">
         <v>17</v>
       </c>
-      <c r="J9" t="s">
-        <v>18</v>
+      <c r="J9" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -1796,7 +1842,7 @@
       <c r="D10" t="s">
         <v>38</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="1" t="s">
         <v>39</v>
       </c>
       <c r="F10" t="s">
@@ -1811,8 +1857,8 @@
       <c r="I10" t="s">
         <v>17</v>
       </c>
-      <c r="J10" t="s">
-        <v>18</v>
+      <c r="J10" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -1828,7 +1874,7 @@
       <c r="D11" t="s">
         <v>41</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F11" t="s">
@@ -1843,8 +1889,8 @@
       <c r="I11" t="s">
         <v>17</v>
       </c>
-      <c r="J11" t="s">
-        <v>18</v>
+      <c r="J11" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -1860,7 +1906,7 @@
       <c r="D12" t="s">
         <v>44</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="1" t="s">
         <v>45</v>
       </c>
       <c r="F12" t="s">
@@ -1875,8 +1921,8 @@
       <c r="I12" t="s">
         <v>17</v>
       </c>
-      <c r="J12" t="s">
-        <v>18</v>
+      <c r="J12" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -1892,7 +1938,7 @@
       <c r="D13" t="s">
         <v>47</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="1" t="s">
         <v>48</v>
       </c>
       <c r="F13" t="s">
@@ -1907,8 +1953,8 @@
       <c r="I13" t="s">
         <v>17</v>
       </c>
-      <c r="J13" t="s">
-        <v>18</v>
+      <c r="J13" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -1924,7 +1970,7 @@
       <c r="D14" t="s">
         <v>47</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="1" t="s">
         <v>48</v>
       </c>
       <c r="F14" t="s">
@@ -1939,8 +1985,8 @@
       <c r="I14" t="s">
         <v>17</v>
       </c>
-      <c r="J14" t="s">
-        <v>18</v>
+      <c r="J14" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -1956,7 +2002,7 @@
       <c r="D15" t="s">
         <v>52</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="1" t="s">
         <v>53</v>
       </c>
       <c r="F15" t="s">
@@ -1971,8 +2017,8 @@
       <c r="I15" t="s">
         <v>17</v>
       </c>
-      <c r="J15" t="s">
-        <v>18</v>
+      <c r="J15" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -1988,7 +2034,7 @@
       <c r="D16" t="s">
         <v>52</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="1" t="s">
         <v>53</v>
       </c>
       <c r="F16" t="s">
@@ -2003,8 +2049,8 @@
       <c r="I16" t="s">
         <v>17</v>
       </c>
-      <c r="J16" t="s">
-        <v>18</v>
+      <c r="J16" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -2020,7 +2066,7 @@
       <c r="D17" t="s">
         <v>56</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="1" t="s">
         <v>57</v>
       </c>
       <c r="F17" t="s">
@@ -2035,8 +2081,8 @@
       <c r="I17" t="s">
         <v>34</v>
       </c>
-      <c r="J17" t="s">
-        <v>18</v>
+      <c r="J17" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -2052,7 +2098,7 @@
       <c r="D18" t="s">
         <v>59</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="1" t="s">
         <v>60</v>
       </c>
       <c r="F18" t="s">
@@ -2067,8 +2113,8 @@
       <c r="I18" t="s">
         <v>26</v>
       </c>
-      <c r="J18" t="s">
-        <v>18</v>
+      <c r="J18" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -2084,7 +2130,7 @@
       <c r="D19" t="s">
         <v>38</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="1" t="s">
         <v>62</v>
       </c>
       <c r="F19" t="s">
@@ -2099,8 +2145,8 @@
       <c r="I19" t="s">
         <v>17</v>
       </c>
-      <c r="J19" t="s">
-        <v>18</v>
+      <c r="J19" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -2116,7 +2162,7 @@
       <c r="D20" t="s">
         <v>38</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="1" t="s">
         <v>62</v>
       </c>
       <c r="F20" t="s">
@@ -2131,8 +2177,8 @@
       <c r="I20" t="s">
         <v>17</v>
       </c>
-      <c r="J20" t="s">
-        <v>18</v>
+      <c r="J20" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -2148,7 +2194,7 @@
       <c r="D21" t="s">
         <v>47</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="1" t="s">
         <v>64</v>
       </c>
       <c r="F21" t="s">
@@ -2163,8 +2209,8 @@
       <c r="I21" t="s">
         <v>17</v>
       </c>
-      <c r="J21" t="s">
-        <v>18</v>
+      <c r="J21" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -2276,7 +2322,7 @@
       <c r="D25" t="s">
         <v>71</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="1" t="s">
         <v>72</v>
       </c>
       <c r="F25" t="s">
@@ -2291,8 +2337,8 @@
       <c r="I25" t="s">
         <v>26</v>
       </c>
-      <c r="J25" t="s">
-        <v>18</v>
+      <c r="J25" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -2308,7 +2354,7 @@
       <c r="D26" t="s">
         <v>47</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="1" t="s">
         <v>74</v>
       </c>
       <c r="F26" t="s">
@@ -2323,8 +2369,8 @@
       <c r="I26" t="s">
         <v>17</v>
       </c>
-      <c r="J26" t="s">
-        <v>18</v>
+      <c r="J26" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
@@ -2340,7 +2386,7 @@
       <c r="D27" t="s">
         <v>47</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="1" t="s">
         <v>74</v>
       </c>
       <c r="F27" t="s">
@@ -2355,8 +2401,8 @@
       <c r="I27" t="s">
         <v>17</v>
       </c>
-      <c r="J27" t="s">
-        <v>18</v>
+      <c r="J27" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -2500,7 +2546,7 @@
       <c r="D32" t="s">
         <v>80</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="1" t="s">
         <v>81</v>
       </c>
       <c r="F32" t="s">
@@ -2515,8 +2561,8 @@
       <c r="I32" t="s">
         <v>26</v>
       </c>
-      <c r="J32" t="s">
-        <v>18</v>
+      <c r="J32" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
@@ -2532,7 +2578,7 @@
       <c r="D33" t="s">
         <v>80</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="1" t="s">
         <v>81</v>
       </c>
       <c r="F33" t="s">
@@ -2547,8 +2593,8 @@
       <c r="I33" t="s">
         <v>26</v>
       </c>
-      <c r="J33" t="s">
-        <v>18</v>
+      <c r="J33" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
@@ -2564,7 +2610,7 @@
       <c r="D34" t="s">
         <v>47</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="1" t="s">
         <v>83</v>
       </c>
       <c r="F34" t="s">
@@ -2579,8 +2625,8 @@
       <c r="I34" t="s">
         <v>17</v>
       </c>
-      <c r="J34" t="s">
-        <v>18</v>
+      <c r="J34" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
@@ -2596,7 +2642,7 @@
       <c r="D35" t="s">
         <v>47</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="1" t="s">
         <v>83</v>
       </c>
       <c r="F35" t="s">
@@ -2611,8 +2657,8 @@
       <c r="I35" t="s">
         <v>17</v>
       </c>
-      <c r="J35" t="s">
-        <v>18</v>
+      <c r="J35" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
@@ -2628,7 +2674,7 @@
       <c r="D36" t="s">
         <v>41</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="1" t="s">
         <v>86</v>
       </c>
       <c r="F36" t="s">
@@ -2643,8 +2689,8 @@
       <c r="I36" t="s">
         <v>17</v>
       </c>
-      <c r="J36" t="s">
-        <v>18</v>
+      <c r="J36" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
@@ -2660,7 +2706,7 @@
       <c r="D37" t="s">
         <v>41</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="1" t="s">
         <v>86</v>
       </c>
       <c r="F37" t="s">
@@ -2675,8 +2721,8 @@
       <c r="I37" t="s">
         <v>17</v>
       </c>
-      <c r="J37" t="s">
-        <v>18</v>
+      <c r="J37" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
@@ -2692,7 +2738,7 @@
       <c r="D38" t="s">
         <v>47</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="1" t="s">
         <v>88</v>
       </c>
       <c r="F38" t="s">
@@ -2707,8 +2753,8 @@
       <c r="I38" t="s">
         <v>17</v>
       </c>
-      <c r="J38" t="s">
-        <v>18</v>
+      <c r="J38" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
@@ -2724,7 +2770,7 @@
       <c r="D39" t="s">
         <v>47</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" s="1" t="s">
         <v>88</v>
       </c>
       <c r="F39" t="s">
@@ -2739,8 +2785,8 @@
       <c r="I39" t="s">
         <v>17</v>
       </c>
-      <c r="J39" t="s">
-        <v>18</v>
+      <c r="J39" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
@@ -2756,7 +2802,7 @@
       <c r="D40" t="s">
         <v>38</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="1" t="s">
         <v>91</v>
       </c>
       <c r="F40" t="s">
@@ -2771,8 +2817,8 @@
       <c r="I40" t="s">
         <v>17</v>
       </c>
-      <c r="J40" t="s">
-        <v>18</v>
+      <c r="J40" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
@@ -2788,7 +2834,7 @@
       <c r="D41" t="s">
         <v>38</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="1" t="s">
         <v>91</v>
       </c>
       <c r="F41" t="s">
@@ -2803,8 +2849,8 @@
       <c r="I41" t="s">
         <v>17</v>
       </c>
-      <c r="J41" t="s">
-        <v>18</v>
+      <c r="J41" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
@@ -2820,7 +2866,7 @@
       <c r="D42" t="s">
         <v>41</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" s="1" t="s">
         <v>93</v>
       </c>
       <c r="F42" t="s">
@@ -2835,8 +2881,8 @@
       <c r="I42" t="s">
         <v>17</v>
       </c>
-      <c r="J42" t="s">
-        <v>18</v>
+      <c r="J42" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
@@ -2852,7 +2898,7 @@
       <c r="D43" t="s">
         <v>41</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E43" s="1" t="s">
         <v>93</v>
       </c>
       <c r="F43" t="s">
@@ -2867,8 +2913,8 @@
       <c r="I43" t="s">
         <v>17</v>
       </c>
-      <c r="J43" t="s">
-        <v>18</v>
+      <c r="J43" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
@@ -2884,7 +2930,7 @@
       <c r="D44" t="s">
         <v>44</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" s="1" t="s">
         <v>95</v>
       </c>
       <c r="F44" t="s">
@@ -2899,8 +2945,8 @@
       <c r="I44" t="s">
         <v>17</v>
       </c>
-      <c r="J44" t="s">
-        <v>18</v>
+      <c r="J44" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
@@ -2916,7 +2962,7 @@
       <c r="D45" t="s">
         <v>44</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E45" s="1" t="s">
         <v>95</v>
       </c>
       <c r="F45" t="s">
@@ -2931,8 +2977,8 @@
       <c r="I45" t="s">
         <v>17</v>
       </c>
-      <c r="J45" t="s">
-        <v>18</v>
+      <c r="J45" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
@@ -2948,7 +2994,7 @@
       <c r="D46" t="s">
         <v>47</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E46" s="1" t="s">
         <v>97</v>
       </c>
       <c r="F46" t="s">
@@ -2963,8 +3009,8 @@
       <c r="I46" t="s">
         <v>17</v>
       </c>
-      <c r="J46" t="s">
-        <v>18</v>
+      <c r="J46" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
@@ -2980,7 +3026,7 @@
       <c r="D47" t="s">
         <v>47</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E47" s="1" t="s">
         <v>97</v>
       </c>
       <c r="F47" t="s">
@@ -2995,8 +3041,8 @@
       <c r="I47" t="s">
         <v>17</v>
       </c>
-      <c r="J47" t="s">
-        <v>18</v>
+      <c r="J47" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
@@ -3012,10 +3058,10 @@
       <c r="D48" t="s">
         <v>99</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E48" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F48" s="1" t="s">
         <v>101</v>
       </c>
       <c r="G48" t="s">
@@ -3027,8 +3073,8 @@
       <c r="I48" t="s">
         <v>17</v>
       </c>
-      <c r="J48" t="s">
-        <v>18</v>
+      <c r="J48" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
@@ -3044,7 +3090,7 @@
       <c r="D49" t="s">
         <v>103</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E49" s="1" t="s">
         <v>104</v>
       </c>
       <c r="F49" t="s">
@@ -3059,8 +3105,8 @@
       <c r="I49" t="s">
         <v>26</v>
       </c>
-      <c r="J49" t="s">
-        <v>18</v>
+      <c r="J49" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
@@ -3076,7 +3122,7 @@
       <c r="D50" t="s">
         <v>80</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E50" s="1" t="s">
         <v>106</v>
       </c>
       <c r="F50" t="s">
@@ -3091,8 +3137,8 @@
       <c r="I50" t="s">
         <v>26</v>
       </c>
-      <c r="J50" t="s">
-        <v>18</v>
+      <c r="J50" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
@@ -3108,7 +3154,7 @@
       <c r="D51" t="s">
         <v>80</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E51" s="1" t="s">
         <v>106</v>
       </c>
       <c r="F51" t="s">
@@ -3123,8 +3169,8 @@
       <c r="I51" t="s">
         <v>26</v>
       </c>
-      <c r="J51" t="s">
-        <v>18</v>
+      <c r="J51" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
@@ -3140,7 +3186,7 @@
       <c r="D52" t="s">
         <v>47</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E52" s="1" t="s">
         <v>108</v>
       </c>
       <c r="F52" t="s">
@@ -3155,8 +3201,8 @@
       <c r="I52" t="s">
         <v>17</v>
       </c>
-      <c r="J52" t="s">
-        <v>18</v>
+      <c r="J52" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
@@ -3172,7 +3218,7 @@
       <c r="D53" t="s">
         <v>47</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E53" s="1" t="s">
         <v>108</v>
       </c>
       <c r="F53" t="s">
@@ -3187,8 +3233,8 @@
       <c r="I53" t="s">
         <v>17</v>
       </c>
-      <c r="J53" t="s">
-        <v>18</v>
+      <c r="J53" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
@@ -3204,10 +3250,10 @@
       <c r="D54" t="s">
         <v>99</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E54" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F54" s="1" t="s">
         <v>111</v>
       </c>
       <c r="G54" t="s">
@@ -3219,8 +3265,8 @@
       <c r="I54" t="s">
         <v>17</v>
       </c>
-      <c r="J54" t="s">
-        <v>18</v>
+      <c r="J54" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
@@ -3300,7 +3346,7 @@
       <c r="D57" t="s">
         <v>47</v>
       </c>
-      <c r="E57" t="s">
+      <c r="E57" s="1" t="s">
         <v>115</v>
       </c>
       <c r="F57" t="s">
@@ -3315,8 +3361,8 @@
       <c r="I57" t="s">
         <v>17</v>
       </c>
-      <c r="J57" t="s">
-        <v>18</v>
+      <c r="J57" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">
@@ -3332,10 +3378,10 @@
       <c r="D58" t="s">
         <v>119</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E58" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="F58" t="s">
+      <c r="F58" s="1" t="s">
         <v>121</v>
       </c>
       <c r="G58" t="s">
@@ -3347,37 +3393,37 @@
       <c r="I58" t="s">
         <v>17</v>
       </c>
-      <c r="J58" t="s">
-        <v>18</v>
+      <c r="J58" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>122</v>
+        <v>161</v>
       </c>
       <c r="B59" t="s">
-        <v>123</v>
+        <v>162</v>
       </c>
       <c r="C59" t="s">
-        <v>55</v>
+        <v>12</v>
       </c>
       <c r="D59" t="s">
-        <v>124</v>
+        <v>163</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>124</v>
+        <v>164</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>125</v>
+        <v>165</v>
       </c>
       <c r="G59" t="s">
         <v>6</v>
       </c>
       <c r="H59" t="s">
-        <v>69</v>
+        <v>16</v>
       </c>
       <c r="I59" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="J59" s="1" t="s">
         <v>160</v>
@@ -3394,25 +3440,25 @@
         <v>55</v>
       </c>
       <c r="D60" t="s">
-        <v>126</v>
-      </c>
-      <c r="E60" t="s">
-        <v>127</v>
-      </c>
-      <c r="F60" t="s">
-        <v>128</v>
+        <v>124</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>125</v>
       </c>
       <c r="G60" t="s">
         <v>6</v>
       </c>
       <c r="H60" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="I60" t="s">
         <v>26</v>
       </c>
-      <c r="J60" t="s">
-        <v>18</v>
+      <c r="J60" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
@@ -3423,16 +3469,16 @@
         <v>123</v>
       </c>
       <c r="C61" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="D61" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E61" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F61" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="G61" t="s">
         <v>6</v>
@@ -3441,7 +3487,7 @@
         <v>16</v>
       </c>
       <c r="I61" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="J61" t="s">
         <v>18</v>
@@ -3455,7 +3501,7 @@
         <v>123</v>
       </c>
       <c r="C62" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="D62" t="s">
         <v>129</v>
@@ -3490,13 +3536,13 @@
         <v>55</v>
       </c>
       <c r="D63" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E63" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F63" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G63" t="s">
         <v>6</v>
@@ -3519,7 +3565,7 @@
         <v>123</v>
       </c>
       <c r="C64" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="D64" t="s">
         <v>132</v>
@@ -3554,13 +3600,13 @@
         <v>37</v>
       </c>
       <c r="D65" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E65" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F65" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G65" t="s">
         <v>6</v>
@@ -3583,7 +3629,7 @@
         <v>123</v>
       </c>
       <c r="C66" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="D66" t="s">
         <v>135</v>
@@ -3615,16 +3661,16 @@
         <v>123</v>
       </c>
       <c r="C67" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="D67" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E67" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F67" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="G67" t="s">
         <v>6</v>
@@ -3641,22 +3687,22 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="B68" t="s">
         <v>123</v>
       </c>
       <c r="C68" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="D68" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="E68" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F68" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G68" t="s">
         <v>6</v>
@@ -3665,7 +3711,7 @@
         <v>16</v>
       </c>
       <c r="I68" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="J68" t="s">
         <v>18</v>
@@ -3679,16 +3725,16 @@
         <v>123</v>
       </c>
       <c r="C69" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="D69" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E69" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F69" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G69" t="s">
         <v>6</v>
@@ -3697,7 +3743,7 @@
         <v>16</v>
       </c>
       <c r="I69" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="J69" t="s">
         <v>18</v>
@@ -3711,16 +3757,16 @@
         <v>123</v>
       </c>
       <c r="C70" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="D70" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E70" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F70" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G70" t="s">
         <v>6</v>
@@ -3743,7 +3789,7 @@
         <v>123</v>
       </c>
       <c r="C71" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="D71" t="s">
         <v>132</v>
@@ -3778,13 +3824,13 @@
         <v>37</v>
       </c>
       <c r="D72" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E72" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F72" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G72" t="s">
         <v>6</v>
@@ -3801,22 +3847,22 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B73" t="s">
         <v>123</v>
       </c>
       <c r="C73" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="D73" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="E73" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F73" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="G73" t="s">
         <v>6</v>
@@ -3842,13 +3888,13 @@
         <v>55</v>
       </c>
       <c r="D74" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E74" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F74" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G74" t="s">
         <v>6</v>
@@ -3871,16 +3917,16 @@
         <v>123</v>
       </c>
       <c r="C75" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D75" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E75" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F75" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G75" t="s">
         <v>6</v>
@@ -3906,24 +3952,56 @@
         <v>51</v>
       </c>
       <c r="D76" t="s">
+        <v>138</v>
+      </c>
+      <c r="E76" t="s">
+        <v>155</v>
+      </c>
+      <c r="F76" t="s">
+        <v>156</v>
+      </c>
+      <c r="G76" t="s">
+        <v>6</v>
+      </c>
+      <c r="H76" t="s">
+        <v>16</v>
+      </c>
+      <c r="I76" t="s">
+        <v>17</v>
+      </c>
+      <c r="J76" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>150</v>
+      </c>
+      <c r="B77" t="s">
+        <v>123</v>
+      </c>
+      <c r="C77" t="s">
+        <v>51</v>
+      </c>
+      <c r="D77" t="s">
         <v>157</v>
       </c>
-      <c r="E76" t="s">
+      <c r="E77" t="s">
         <v>158</v>
       </c>
-      <c r="F76" t="s">
+      <c r="F77" t="s">
         <v>159</v>
       </c>
-      <c r="G76" t="s">
-        <v>6</v>
-      </c>
-      <c r="H76" t="s">
-        <v>16</v>
-      </c>
-      <c r="I76" t="s">
-        <v>17</v>
-      </c>
-      <c r="J76" t="s">
+      <c r="G77" t="s">
+        <v>6</v>
+      </c>
+      <c r="H77" t="s">
+        <v>16</v>
+      </c>
+      <c r="I77" t="s">
+        <v>17</v>
+      </c>
+      <c r="J77" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Compile list of manually checked SpeciesSeeded column, but there might be duplicates and those need addressing
</commit_message>
<xml_diff>
--- a/data/raw/03.1b_edited-species-seeded1_corrected-seeded-not-in-mix_subplot.xlsx
+++ b/data/raw/03.1b_edited-species-seeded1_corrected-seeded-not-in-mix_subplot.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="104" documentId="13_ncr:40009_{E4B6624F-F1D1-4948-BE4F-D27FFF9DA9DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8EA6864-194B-40E0-B1E6-F75F26780712}"/>
+  <xr:revisionPtr revIDLastSave="171" documentId="13_ncr:40009_{E4B6624F-F1D1-4948-BE4F-D27FFF9DA9DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD09FA6D-D917-404E-AF38-AE8EBC865E73}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -22,10 +22,10 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={B2899F8C-4835-4657-A201-9626AE43BAA8}</author>
+    <author>tc={A6CD19F4-2BA9-431F-95D0-FCCA0F4BBCEC}</author>
   </authors>
   <commentList>
-    <comment ref="E60" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="E60" authorId="0" shapeId="0" xr:uid="{A6CD19F4-2BA9-431F-95D0-FCCA0F4BBCEC}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1106,7 +1106,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AA59FCB-323B-ADC5-C9D5-9E8A9228024C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE1D0C3D-2187-4904-B798-BAC09FEA6563}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1114,8 +1114,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11729084" y="567690"/>
-          <a:ext cx="3560445" cy="3072765"/>
+          <a:off x="11727179" y="563880"/>
+          <a:ext cx="3564255" cy="3072765"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1168,12 +1168,6 @@
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
             <a:t>- Named "local Bouteloua" because if it's local I think that implies a volunteer, and also because the same name was used at other sites and marked not seeded. </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>- Marked "Yes?" - I just took away question mark.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1514,19 +1508,19 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="E60" dT="2023-09-07T00:11:45.05" personId="{8230C25F-1289-450E-882A-C133D8E3F471}" id="{B2899F8C-4835-4657-A201-9626AE43BAA8}">
+  <threadedComment ref="E60" dT="2023-09-07T00:11:45.05" personId="{8230C25F-1289-450E-882A-C133D8E3F471}" id="{A6CD19F4-2BA9-431F-95D0-FCCA0F4BBCEC}">
     <text>USDA code is actually LILE29</text>
   </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05C66056-BDB3-4C93-9739-661D41665B2E}">
   <dimension ref="A1:J77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J57" sqref="J57"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1586,7 +1580,7 @@
       <c r="D2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>14</v>
       </c>
       <c r="F2" t="s">
@@ -1601,8 +1595,8 @@
       <c r="I2" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>160</v>
+      <c r="J2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -1618,7 +1612,7 @@
       <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
         <v>14</v>
       </c>
       <c r="F3" t="s">
@@ -1633,8 +1627,8 @@
       <c r="I3" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>160</v>
+      <c r="J3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -1650,7 +1644,7 @@
       <c r="D4" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>21</v>
       </c>
       <c r="F4" t="s">
@@ -1665,8 +1659,8 @@
       <c r="I4" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>160</v>
+      <c r="J4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -1682,7 +1676,7 @@
       <c r="D5" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>24</v>
       </c>
       <c r="F5" t="s">
@@ -1697,8 +1691,8 @@
       <c r="I5" t="s">
         <v>26</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>160</v>
+      <c r="J5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -1714,7 +1708,7 @@
       <c r="D6" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>28</v>
       </c>
       <c r="F6" t="s">
@@ -1729,8 +1723,8 @@
       <c r="I6" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>160</v>
+      <c r="J6" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -1746,7 +1740,7 @@
       <c r="D7" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
         <v>28</v>
       </c>
       <c r="F7" t="s">
@@ -1761,8 +1755,8 @@
       <c r="I7" t="s">
         <v>17</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>160</v>
+      <c r="J7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -1778,7 +1772,7 @@
       <c r="D8" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" t="s">
         <v>31</v>
       </c>
       <c r="F8" t="s">
@@ -1793,8 +1787,8 @@
       <c r="I8" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>160</v>
+      <c r="J8" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -1810,7 +1804,7 @@
       <c r="D9" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
         <v>39</v>
       </c>
       <c r="F9" t="s">
@@ -1825,8 +1819,8 @@
       <c r="I9" t="s">
         <v>17</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>160</v>
+      <c r="J9" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -1842,7 +1836,7 @@
       <c r="D10" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" t="s">
         <v>39</v>
       </c>
       <c r="F10" t="s">
@@ -1857,8 +1851,8 @@
       <c r="I10" t="s">
         <v>17</v>
       </c>
-      <c r="J10" s="1" t="s">
-        <v>160</v>
+      <c r="J10" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -1874,7 +1868,7 @@
       <c r="D11" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" t="s">
         <v>42</v>
       </c>
       <c r="F11" t="s">
@@ -1889,8 +1883,8 @@
       <c r="I11" t="s">
         <v>17</v>
       </c>
-      <c r="J11" s="1" t="s">
-        <v>160</v>
+      <c r="J11" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -1906,7 +1900,7 @@
       <c r="D12" t="s">
         <v>44</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" t="s">
         <v>45</v>
       </c>
       <c r="F12" t="s">
@@ -1921,8 +1915,8 @@
       <c r="I12" t="s">
         <v>17</v>
       </c>
-      <c r="J12" s="1" t="s">
-        <v>160</v>
+      <c r="J12" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -1938,7 +1932,7 @@
       <c r="D13" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" t="s">
         <v>48</v>
       </c>
       <c r="F13" t="s">
@@ -1953,8 +1947,8 @@
       <c r="I13" t="s">
         <v>17</v>
       </c>
-      <c r="J13" s="1" t="s">
-        <v>160</v>
+      <c r="J13" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -1970,7 +1964,7 @@
       <c r="D14" t="s">
         <v>47</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" t="s">
         <v>48</v>
       </c>
       <c r="F14" t="s">
@@ -1985,8 +1979,8 @@
       <c r="I14" t="s">
         <v>17</v>
       </c>
-      <c r="J14" s="1" t="s">
-        <v>160</v>
+      <c r="J14" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -2002,7 +1996,7 @@
       <c r="D15" t="s">
         <v>52</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" t="s">
         <v>53</v>
       </c>
       <c r="F15" t="s">
@@ -2017,8 +2011,8 @@
       <c r="I15" t="s">
         <v>17</v>
       </c>
-      <c r="J15" s="1" t="s">
-        <v>160</v>
+      <c r="J15" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -2034,7 +2028,7 @@
       <c r="D16" t="s">
         <v>52</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" t="s">
         <v>53</v>
       </c>
       <c r="F16" t="s">
@@ -2049,8 +2043,8 @@
       <c r="I16" t="s">
         <v>17</v>
       </c>
-      <c r="J16" s="1" t="s">
-        <v>160</v>
+      <c r="J16" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -2066,7 +2060,7 @@
       <c r="D17" t="s">
         <v>56</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" t="s">
         <v>57</v>
       </c>
       <c r="F17" t="s">
@@ -2079,10 +2073,10 @@
         <v>16</v>
       </c>
       <c r="I17" t="s">
-        <v>34</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>160</v>
+        <v>17</v>
+      </c>
+      <c r="J17" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -2098,7 +2092,7 @@
       <c r="D18" t="s">
         <v>59</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" t="s">
         <v>60</v>
       </c>
       <c r="F18" t="s">
@@ -2113,8 +2107,8 @@
       <c r="I18" t="s">
         <v>26</v>
       </c>
-      <c r="J18" s="1" t="s">
-        <v>160</v>
+      <c r="J18" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -2130,7 +2124,7 @@
       <c r="D19" t="s">
         <v>38</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" t="s">
         <v>62</v>
       </c>
       <c r="F19" t="s">
@@ -2145,8 +2139,8 @@
       <c r="I19" t="s">
         <v>17</v>
       </c>
-      <c r="J19" s="1" t="s">
-        <v>160</v>
+      <c r="J19" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -2162,7 +2156,7 @@
       <c r="D20" t="s">
         <v>38</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" t="s">
         <v>62</v>
       </c>
       <c r="F20" t="s">
@@ -2177,8 +2171,8 @@
       <c r="I20" t="s">
         <v>17</v>
       </c>
-      <c r="J20" s="1" t="s">
-        <v>160</v>
+      <c r="J20" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -2194,7 +2188,7 @@
       <c r="D21" t="s">
         <v>47</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" t="s">
         <v>64</v>
       </c>
       <c r="F21" t="s">
@@ -2209,8 +2203,8 @@
       <c r="I21" t="s">
         <v>17</v>
       </c>
-      <c r="J21" s="1" t="s">
-        <v>160</v>
+      <c r="J21" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -2322,7 +2316,7 @@
       <c r="D25" t="s">
         <v>71</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" t="s">
         <v>72</v>
       </c>
       <c r="F25" t="s">
@@ -2337,8 +2331,8 @@
       <c r="I25" t="s">
         <v>26</v>
       </c>
-      <c r="J25" s="1" t="s">
-        <v>160</v>
+      <c r="J25" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -2354,7 +2348,7 @@
       <c r="D26" t="s">
         <v>47</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" t="s">
         <v>74</v>
       </c>
       <c r="F26" t="s">
@@ -2369,8 +2363,8 @@
       <c r="I26" t="s">
         <v>17</v>
       </c>
-      <c r="J26" s="1" t="s">
-        <v>160</v>
+      <c r="J26" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
@@ -2386,7 +2380,7 @@
       <c r="D27" t="s">
         <v>47</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" t="s">
         <v>74</v>
       </c>
       <c r="F27" t="s">
@@ -2401,8 +2395,8 @@
       <c r="I27" t="s">
         <v>17</v>
       </c>
-      <c r="J27" s="1" t="s">
-        <v>160</v>
+      <c r="J27" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -2546,7 +2540,7 @@
       <c r="D32" t="s">
         <v>80</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" t="s">
         <v>81</v>
       </c>
       <c r="F32" t="s">
@@ -2561,8 +2555,8 @@
       <c r="I32" t="s">
         <v>26</v>
       </c>
-      <c r="J32" s="1" t="s">
-        <v>160</v>
+      <c r="J32" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
@@ -2578,7 +2572,7 @@
       <c r="D33" t="s">
         <v>80</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E33" t="s">
         <v>81</v>
       </c>
       <c r="F33" t="s">
@@ -2593,8 +2587,8 @@
       <c r="I33" t="s">
         <v>26</v>
       </c>
-      <c r="J33" s="1" t="s">
-        <v>160</v>
+      <c r="J33" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
@@ -2610,7 +2604,7 @@
       <c r="D34" t="s">
         <v>47</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E34" t="s">
         <v>83</v>
       </c>
       <c r="F34" t="s">
@@ -2625,8 +2619,8 @@
       <c r="I34" t="s">
         <v>17</v>
       </c>
-      <c r="J34" s="1" t="s">
-        <v>160</v>
+      <c r="J34" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
@@ -2642,7 +2636,7 @@
       <c r="D35" t="s">
         <v>47</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E35" t="s">
         <v>83</v>
       </c>
       <c r="F35" t="s">
@@ -2657,8 +2651,8 @@
       <c r="I35" t="s">
         <v>17</v>
       </c>
-      <c r="J35" s="1" t="s">
-        <v>160</v>
+      <c r="J35" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
@@ -2674,7 +2668,7 @@
       <c r="D36" t="s">
         <v>41</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E36" t="s">
         <v>86</v>
       </c>
       <c r="F36" t="s">
@@ -2689,8 +2683,8 @@
       <c r="I36" t="s">
         <v>17</v>
       </c>
-      <c r="J36" s="1" t="s">
-        <v>160</v>
+      <c r="J36" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
@@ -2706,7 +2700,7 @@
       <c r="D37" t="s">
         <v>41</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E37" t="s">
         <v>86</v>
       </c>
       <c r="F37" t="s">
@@ -2721,8 +2715,8 @@
       <c r="I37" t="s">
         <v>17</v>
       </c>
-      <c r="J37" s="1" t="s">
-        <v>160</v>
+      <c r="J37" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
@@ -2738,7 +2732,7 @@
       <c r="D38" t="s">
         <v>47</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E38" t="s">
         <v>88</v>
       </c>
       <c r="F38" t="s">
@@ -2753,8 +2747,8 @@
       <c r="I38" t="s">
         <v>17</v>
       </c>
-      <c r="J38" s="1" t="s">
-        <v>160</v>
+      <c r="J38" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
@@ -2770,7 +2764,7 @@
       <c r="D39" t="s">
         <v>47</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E39" t="s">
         <v>88</v>
       </c>
       <c r="F39" t="s">
@@ -2785,8 +2779,8 @@
       <c r="I39" t="s">
         <v>17</v>
       </c>
-      <c r="J39" s="1" t="s">
-        <v>160</v>
+      <c r="J39" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
@@ -2802,7 +2796,7 @@
       <c r="D40" t="s">
         <v>38</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E40" t="s">
         <v>91</v>
       </c>
       <c r="F40" t="s">
@@ -2817,8 +2811,8 @@
       <c r="I40" t="s">
         <v>17</v>
       </c>
-      <c r="J40" s="1" t="s">
-        <v>160</v>
+      <c r="J40" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
@@ -2834,7 +2828,7 @@
       <c r="D41" t="s">
         <v>38</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E41" t="s">
         <v>91</v>
       </c>
       <c r="F41" t="s">
@@ -2849,8 +2843,8 @@
       <c r="I41" t="s">
         <v>17</v>
       </c>
-      <c r="J41" s="1" t="s">
-        <v>160</v>
+      <c r="J41" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
@@ -2866,7 +2860,7 @@
       <c r="D42" t="s">
         <v>41</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E42" t="s">
         <v>93</v>
       </c>
       <c r="F42" t="s">
@@ -2881,8 +2875,8 @@
       <c r="I42" t="s">
         <v>17</v>
       </c>
-      <c r="J42" s="1" t="s">
-        <v>160</v>
+      <c r="J42" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
@@ -2898,7 +2892,7 @@
       <c r="D43" t="s">
         <v>41</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E43" t="s">
         <v>93</v>
       </c>
       <c r="F43" t="s">
@@ -2913,8 +2907,8 @@
       <c r="I43" t="s">
         <v>17</v>
       </c>
-      <c r="J43" s="1" t="s">
-        <v>160</v>
+      <c r="J43" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
@@ -2930,7 +2924,7 @@
       <c r="D44" t="s">
         <v>44</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="E44" t="s">
         <v>95</v>
       </c>
       <c r="F44" t="s">
@@ -2945,8 +2939,8 @@
       <c r="I44" t="s">
         <v>17</v>
       </c>
-      <c r="J44" s="1" t="s">
-        <v>160</v>
+      <c r="J44" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
@@ -2962,7 +2956,7 @@
       <c r="D45" t="s">
         <v>44</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E45" t="s">
         <v>95</v>
       </c>
       <c r="F45" t="s">
@@ -2977,8 +2971,8 @@
       <c r="I45" t="s">
         <v>17</v>
       </c>
-      <c r="J45" s="1" t="s">
-        <v>160</v>
+      <c r="J45" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
@@ -2994,7 +2988,7 @@
       <c r="D46" t="s">
         <v>47</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="E46" t="s">
         <v>97</v>
       </c>
       <c r="F46" t="s">
@@ -3009,8 +3003,8 @@
       <c r="I46" t="s">
         <v>17</v>
       </c>
-      <c r="J46" s="1" t="s">
-        <v>160</v>
+      <c r="J46" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
@@ -3026,7 +3020,7 @@
       <c r="D47" t="s">
         <v>47</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="E47" t="s">
         <v>97</v>
       </c>
       <c r="F47" t="s">
@@ -3041,8 +3035,8 @@
       <c r="I47" t="s">
         <v>17</v>
       </c>
-      <c r="J47" s="1" t="s">
-        <v>160</v>
+      <c r="J47" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
@@ -3090,7 +3084,7 @@
       <c r="D49" t="s">
         <v>103</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="E49" t="s">
         <v>104</v>
       </c>
       <c r="F49" t="s">
@@ -3105,8 +3099,8 @@
       <c r="I49" t="s">
         <v>26</v>
       </c>
-      <c r="J49" s="1" t="s">
-        <v>160</v>
+      <c r="J49" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
@@ -3122,7 +3116,7 @@
       <c r="D50" t="s">
         <v>80</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="E50" t="s">
         <v>106</v>
       </c>
       <c r="F50" t="s">
@@ -3137,8 +3131,8 @@
       <c r="I50" t="s">
         <v>26</v>
       </c>
-      <c r="J50" s="1" t="s">
-        <v>160</v>
+      <c r="J50" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
@@ -3154,7 +3148,7 @@
       <c r="D51" t="s">
         <v>80</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="E51" t="s">
         <v>106</v>
       </c>
       <c r="F51" t="s">
@@ -3169,8 +3163,8 @@
       <c r="I51" t="s">
         <v>26</v>
       </c>
-      <c r="J51" s="1" t="s">
-        <v>160</v>
+      <c r="J51" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
@@ -3186,7 +3180,7 @@
       <c r="D52" t="s">
         <v>47</v>
       </c>
-      <c r="E52" s="1" t="s">
+      <c r="E52" t="s">
         <v>108</v>
       </c>
       <c r="F52" t="s">
@@ -3201,8 +3195,8 @@
       <c r="I52" t="s">
         <v>17</v>
       </c>
-      <c r="J52" s="1" t="s">
-        <v>160</v>
+      <c r="J52" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
@@ -3218,7 +3212,7 @@
       <c r="D53" t="s">
         <v>47</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="E53" t="s">
         <v>108</v>
       </c>
       <c r="F53" t="s">
@@ -3233,8 +3227,8 @@
       <c r="I53" t="s">
         <v>17</v>
       </c>
-      <c r="J53" s="1" t="s">
-        <v>160</v>
+      <c r="J53" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
@@ -3346,7 +3340,7 @@
       <c r="D57" t="s">
         <v>47</v>
       </c>
-      <c r="E57" s="1" t="s">
+      <c r="E57" t="s">
         <v>115</v>
       </c>
       <c r="F57" t="s">
@@ -3361,8 +3355,8 @@
       <c r="I57" t="s">
         <v>17</v>
       </c>
-      <c r="J57" s="1" t="s">
-        <v>160</v>
+      <c r="J57" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>